<commit_message>
Updated with names for Jan month
</commit_message>
<xml_diff>
--- a/Monthly_status_update.xlsx
+++ b/Monthly_status_update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,23 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Nitesh</t>
+  </si>
+  <si>
+    <t>Gautami</t>
+  </si>
+  <si>
+    <t>Pratiksha</t>
+  </si>
+  <si>
+    <t>Pruthvi</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +359,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -370,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Removed tasks for Feb
</commit_message>
<xml_diff>
--- a/Monthly_status_update.xlsx
+++ b/Monthly_status_update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Nitesh</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,36 +432,24 @@
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
+    </row>
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>